<commit_message>
fix & add Codebook 4.
</commit_message>
<xml_diff>
--- a/Projects/blubbi90/StandardOperatingProcedureLayout/Datasets/codebooks/7. Verpacken.xlsx
+++ b/Projects/blubbi90/StandardOperatingProcedureLayout/Datasets/codebooks/7. Verpacken.xlsx
@@ -374,12 +374,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -578,7 +578,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,7 +588,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -603,72 +603,72 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>